<commit_message>
add grant, adjust content
</commit_message>
<xml_diff>
--- a/positions.xlsx
+++ b/positions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\cv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B32056A-F160-4837-9FDD-5BAE941FE241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BBBF9F-578F-45E5-AB0C-7D5D30F16F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="157">
   <si>
     <t># education</t>
   </si>
@@ -207,21 +207,9 @@
     <t>优秀毕业研究生</t>
   </si>
   <si>
-    <t>#"**PI**</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CNY ¥1</t>
-  </si>
-  <si>
     <t>grant</t>
   </si>
   <si>
-    <t xml:space="preserve"> CNY ¥100</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CNY ¥20</t>
-  </si>
-  <si>
     <t>中国土壤学会第十三次全国会员代表大会</t>
   </si>
   <si>
@@ -243,9 +231,6 @@
     <t>上海</t>
   </si>
   <si>
-    <t>华中农业大学资源与环境学院博士后交流会</t>
-  </si>
-  <si>
     <t>细菌的江湖——土壤微生物互作研究</t>
   </si>
   <si>
@@ -536,6 +521,54 @@
   </si>
   <si>
     <t># _present_</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国家重点研发计划子课题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>博士后基金面上项目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NSFC 青年科学基金</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> CNY ¥5（主持）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> CNY ¥72.5（主持）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> CNY ¥24（主持）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># 华中农业大学资源与环境学院博士后交流会</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -866,7 +899,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -929,10 +962,10 @@
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
         <v>21</v>
@@ -961,10 +994,10 @@
         <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
         <v>25</v>
@@ -993,10 +1026,10 @@
         <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
@@ -1021,22 +1054,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I7" t="s">
         <v>33</v>
@@ -1053,10 +1086,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
@@ -1085,10 +1118,10 @@
         <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
@@ -1117,10 +1150,10 @@
         <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
@@ -1154,10 +1187,10 @@
         <v>42</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F12" t="s">
         <v>22</v>
@@ -1186,10 +1219,10 @@
         <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F13" t="s">
         <v>22</v>
@@ -1218,10 +1251,10 @@
         <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F14" t="s">
         <v>22</v>
@@ -1241,7 +1274,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B15" t="s">
         <v>48</v>
@@ -1250,10 +1283,10 @@
         <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
@@ -1539,31 +1572,31 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" t="s">
         <v>60</v>
-      </c>
-      <c r="B26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2018</v>
-      </c>
-      <c r="E26" s="1">
-        <v>2020</v>
-      </c>
-      <c r="F26" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H26" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" t="s">
-        <v>62</v>
       </c>
       <c r="J26" t="s">
         <v>22</v>
@@ -1571,31 +1604,31 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" t="s">
         <v>60</v>
-      </c>
-      <c r="B27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="1">
-        <v>2013</v>
-      </c>
-      <c r="E27" s="1">
-        <v>2013</v>
-      </c>
-      <c r="F27" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" t="s">
-        <v>62</v>
       </c>
       <c r="J27" t="s">
         <v>22</v>
@@ -1603,31 +1636,31 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" t="s">
         <v>60</v>
-      </c>
-      <c r="B28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="1">
-        <v>2011</v>
-      </c>
-      <c r="E28" s="1">
-        <v>2011</v>
-      </c>
-      <c r="F28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" t="s">
-        <v>62</v>
       </c>
       <c r="J28" t="s">
         <v>22</v>
@@ -1640,13 +1673,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D30" s="1">
         <v>2016</v>
@@ -1664,7 +1697,7 @@
         <v>22</v>
       </c>
       <c r="I30" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J30" t="s">
         <v>22</v>
@@ -1672,13 +1705,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D31" s="1">
         <v>2017</v>
@@ -1696,7 +1729,7 @@
         <v>22</v>
       </c>
       <c r="I31" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J31" t="s">
         <v>22</v>
@@ -1704,19 +1737,19 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>156</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
         <v>42</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F32" t="s">
         <v>22</v>
@@ -1728,7 +1761,7 @@
         <v>22</v>
       </c>
       <c r="I32" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J32" t="s">
         <v>22</v>
@@ -1736,66 +1769,66 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F33" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G33" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H33" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J33" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" t="s">
+        <v>96</v>
+      </c>
+      <c r="G34" t="s">
+        <v>96</v>
+      </c>
+      <c r="H34" t="s">
+        <v>96</v>
+      </c>
+      <c r="I34" t="s">
         <v>131</v>
       </c>
-      <c r="B34" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" t="s">
-        <v>133</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F34" t="s">
-        <v>101</v>
-      </c>
-      <c r="G34" t="s">
-        <v>101</v>
-      </c>
-      <c r="H34" t="s">
-        <v>101</v>
-      </c>
-      <c r="I34" t="s">
-        <v>136</v>
-      </c>
       <c r="J34" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.4">
@@ -1805,19 +1838,19 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
         <v>30</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F36" t="s">
         <v>22</v>
@@ -1829,7 +1862,7 @@
         <v>22</v>
       </c>
       <c r="I36" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J36" t="s">
         <v>22</v>
@@ -1842,19 +1875,19 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F38" t="s">
         <v>22</v>
@@ -1866,7 +1899,7 @@
         <v>22</v>
       </c>
       <c r="I38" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J38" t="s">
         <v>22</v>
@@ -1874,19 +1907,19 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F39" t="s">
         <v>22</v>
@@ -1898,7 +1931,7 @@
         <v>22</v>
       </c>
       <c r="I39" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J39" t="s">
         <v>22</v>
@@ -1906,19 +1939,19 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
         <v>20</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F40" t="s">
         <v>22</v>
@@ -1930,7 +1963,7 @@
         <v>22</v>
       </c>
       <c r="I40" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J40" t="s">
         <v>22</v>
@@ -1938,19 +1971,19 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B41" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C41" t="s">
         <v>20</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F41" t="s">
         <v>22</v>
@@ -1962,7 +1995,7 @@
         <v>22</v>
       </c>
       <c r="I41" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J41" t="s">
         <v>22</v>
@@ -1970,19 +2003,19 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" t="s">
         <v>77</v>
       </c>
-      <c r="B42" t="s">
-        <v>82</v>
-      </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F42" t="s">
         <v>22</v>
@@ -1994,7 +2027,7 @@
         <v>22</v>
       </c>
       <c r="I42" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J42" t="s">
         <v>22</v>
@@ -2002,19 +2035,19 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F43" t="s">
         <v>22</v>
@@ -2026,7 +2059,7 @@
         <v>22</v>
       </c>
       <c r="I43" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J43" t="s">
         <v>22</v>
@@ -2034,19 +2067,19 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B44" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F44" t="s">
         <v>22</v>
@@ -2058,7 +2091,7 @@
         <v>22</v>
       </c>
       <c r="I44" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J44" t="s">
         <v>22</v>
@@ -2066,7 +2099,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
         <v>29</v>
@@ -2075,10 +2108,10 @@
         <v>30</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F45" t="s">
         <v>22</v>
@@ -2090,7 +2123,7 @@
         <v>22</v>
       </c>
       <c r="I45" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J45" t="s">
         <v>22</v>
@@ -2098,19 +2131,19 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C46" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F46" t="s">
         <v>22</v>
@@ -2122,7 +2155,7 @@
         <v>22</v>
       </c>
       <c r="I46" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J46" t="s">
         <v>22</v>
@@ -2130,34 +2163,34 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B47" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C47" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F47" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G47" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H47" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I47" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="J47" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update position, adjust research summary
</commit_message>
<xml_diff>
--- a/positions.xlsx
+++ b/positions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\cv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C027E4-83C0-4BB8-BAA2-AA6EFFB5C922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C6DD1F-58AC-4B59-A58B-8A41DBA1FE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="165">
   <si>
     <t># education</t>
   </si>
@@ -274,14 +274,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>北京热心肠生物技术研究院有限公司</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>北京, 中国</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Shaoshan, CN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -560,10 +552,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> CNY ¥24（主持）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>无序化结构在分枝杆菌广泛调节因子中的功能（2013M541836）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -577,6 +565,41 @@
   </si>
   <si>
     <t>微生物种间相互作用的微生态机制（项目号：2016YFD0800206）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021-10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beijing Rexinchang Biotechnology Research Institute Co. Ltd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beijing, CN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Associate Professor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021-11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> CNY ¥30（主持）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>International Symposium on Multiscale Biofilm Interfacial Processes and Soil Health</t>
+  </si>
+  <si>
+    <t>Session host</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021-12-15</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -903,11 +926,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -961,22 +984,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
@@ -996,19 +1019,19 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
@@ -1025,22 +1048,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
         <v>22</v>
@@ -1062,74 +1085,77 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>159</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
       </c>
       <c r="I7" t="s">
         <v>33</v>
       </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>157</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>158</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="I8" t="s">
         <v>33</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
@@ -1149,13 +1175,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>114</v>
@@ -1181,56 +1207,56 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J12" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F13" t="s">
         <v>22</v>
@@ -1250,19 +1276,19 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F14" t="s">
         <v>22</v>
@@ -1282,19 +1308,19 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
@@ -1314,56 +1340,56 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>141</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="1">
-        <v>2004</v>
-      </c>
-      <c r="E17" s="1">
-        <v>2005</v>
-      </c>
-      <c r="F17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="1">
+        <v>2004</v>
+      </c>
+      <c r="E18" s="1">
         <v>2005</v>
-      </c>
-      <c r="E18" s="1">
-        <v>2006</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
@@ -1383,19 +1409,19 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="1">
+        <v>2005</v>
+      </c>
+      <c r="E19" s="1">
         <v>2006</v>
-      </c>
-      <c r="E19" s="1">
-        <v>2007</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
@@ -1415,19 +1441,19 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="1">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="E20" s="1">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="F20" t="s">
         <v>22</v>
@@ -1447,10 +1473,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
@@ -1459,7 +1485,7 @@
         <v>2008</v>
       </c>
       <c r="E21" s="1">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="F21" t="s">
         <v>22</v>
@@ -1488,10 +1514,10 @@
         <v>20</v>
       </c>
       <c r="D22" s="1">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="E22" s="1">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="F22" t="s">
         <v>22</v>
@@ -1511,19 +1537,19 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E23" s="1">
         <v>2011</v>
-      </c>
-      <c r="E23" s="1">
-        <v>2012</v>
       </c>
       <c r="F23" t="s">
         <v>22</v>
@@ -1543,16 +1569,16 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="1">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="E24" s="1">
         <v>2012</v>
@@ -1575,59 +1601,59 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2012</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" t="s">
+        <v>51</v>
+      </c>
+      <c r="J25" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>147</v>
-      </c>
-      <c r="B26" t="s">
-        <v>152</v>
-      </c>
-      <c r="C26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F26" t="s">
-        <v>155</v>
-      </c>
-      <c r="G26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H26" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" t="s">
-        <v>60</v>
-      </c>
-      <c r="J26" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B27" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C27" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="F27" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="G27" t="s">
         <v>22</v>
@@ -1644,22 +1670,22 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B28" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C28" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="F28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G28" t="s">
         <v>22</v>
@@ -1676,88 +1702,88 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>146</v>
+      </c>
+      <c r="B29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F29" t="s">
+        <v>153</v>
+      </c>
+      <c r="G29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" t="s">
+        <v>60</v>
+      </c>
+      <c r="J29" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E30" s="1">
-        <v>2016</v>
-      </c>
-      <c r="F30" t="s">
-        <v>22</v>
-      </c>
-      <c r="G30" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I30" t="s">
-        <v>64</v>
-      </c>
-      <c r="J30" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>162</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>163</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E31" s="1">
-        <v>2017</v>
+        <v>81</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="F31" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="G31" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="H31" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="I31" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="J31" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>85</v>
+        <v>63</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2016</v>
       </c>
       <c r="F32" t="s">
         <v>22</v>
@@ -1777,125 +1803,152 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>104</v>
+        <v>67</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2017</v>
       </c>
       <c r="F33" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="G33" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="H33" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="I33" t="s">
         <v>64</v>
       </c>
       <c r="J33" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>128</v>
+        <v>42</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
       <c r="F34" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="G34" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="H34" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="I34" t="s">
-        <v>131</v>
+        <v>64</v>
       </c>
       <c r="J34" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>98</v>
+      </c>
+      <c r="B35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F35" t="s">
+        <v>94</v>
+      </c>
+      <c r="G35" t="s">
+        <v>94</v>
+      </c>
+      <c r="H35" t="s">
+        <v>94</v>
+      </c>
+      <c r="I35" t="s">
+        <v>64</v>
+      </c>
+      <c r="J35" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>86</v>
+        <v>127</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="F36" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="G36" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="H36" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="I36" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="J36" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>138</v>
+        <v>70</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F38" t="s">
         <v>22</v>
@@ -1907,7 +1960,7 @@
         <v>22</v>
       </c>
       <c r="I38" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J38" t="s">
         <v>22</v>
@@ -1915,34 +1968,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>132</v>
-      </c>
-      <c r="B39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F39" t="s">
-        <v>22</v>
-      </c>
-      <c r="G39" t="s">
-        <v>22</v>
-      </c>
-      <c r="H39" t="s">
-        <v>22</v>
-      </c>
-      <c r="I39" t="s">
-        <v>74</v>
-      </c>
-      <c r="J39" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.4">
@@ -1950,16 +1976,16 @@
         <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
       <c r="C40" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F40" t="s">
         <v>22</v>
@@ -1979,19 +2005,19 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B41" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F41" t="s">
         <v>22</v>
@@ -2014,16 +2040,16 @@
         <v>72</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F42" t="s">
         <v>22</v>
@@ -2043,19 +2069,19 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>135</v>
       </c>
       <c r="C43" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F43" t="s">
         <v>22</v>
@@ -2078,16 +2104,16 @@
         <v>72</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="C44" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="F44" t="s">
         <v>22</v>
@@ -2107,19 +2133,19 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="C45" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="F45" t="s">
         <v>22</v>
@@ -2139,19 +2165,19 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>72</v>
       </c>
       <c r="B46" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="C46" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="F46" t="s">
         <v>22</v>
@@ -2171,34 +2197,98 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F47" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" t="s">
+        <v>74</v>
+      </c>
+      <c r="J47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>130</v>
+      </c>
+      <c r="B48" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" t="s">
+        <v>131</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B47" t="s">
-        <v>142</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="F48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48" t="s">
+        <v>74</v>
+      </c>
+      <c r="J48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" t="s">
+        <v>140</v>
+      </c>
+      <c r="C49" t="s">
         <v>81</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D49" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F49" t="s">
+        <v>94</v>
+      </c>
+      <c r="G49" t="s">
+        <v>94</v>
+      </c>
+      <c r="H49" t="s">
+        <v>94</v>
+      </c>
+      <c r="I49" t="s">
         <v>139</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F47" t="s">
-        <v>96</v>
-      </c>
-      <c r="G47" t="s">
-        <v>96</v>
-      </c>
-      <c r="H47" t="s">
-        <v>96</v>
-      </c>
-      <c r="I47" t="s">
-        <v>141</v>
-      </c>
-      <c r="J47" t="s">
-        <v>96</v>
+      <c r="J49" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>